<commit_message>
added files documenting design and proof of flask endpoints to sprint 8 assets folder
</commit_message>
<xml_diff>
--- a/project_management/flask_apis.xlsx
+++ b/project_management/flask_apis.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Grego\Desktop\Coding\Projects\plan_tool\project_management\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBA7596A-47A4-4A69-A26C-388AD04FBBCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F8D781A-CF6D-4D82-81C6-BC75F98BC9B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{C551EE5F-BC6E-4444-BA40-FE73DEA46AED}"/>
   </bookViews>
   <sheets>
     <sheet name="api_doc" sheetId="4" r:id="rId1"/>
     <sheet name="design_1" sheetId="5" r:id="rId2"/>
+    <sheet name="stats_data_example" sheetId="7" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="62">
   <si>
     <t>Method</t>
   </si>
@@ -502,7 +503,140 @@
     <t>Request statistical metric calculations that will filter work records based on the start and end date values passed (inclusive)</t>
   </si>
   <si>
-    <t>{ "wor": true, "service": "flask", "version": "x.y.z", "now": "2025-08-23T17:02:00Z" }</t>
+    <t>{</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "day": {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    "ave": {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      "Fri": 396.25,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      "Mon": 423.0,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      "Sat": 360.25,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      "Sun": 473.25,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      "Thu": 355.25,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      "Tue": 327.5,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      "Wed": 357.25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    },</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    "std": {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      "Fri": 88.20572543775148,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      "Mon": 44.7288124888943,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      "Sat": 131.98832801933603,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      "Sun": 120.4778679536896,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      "Thu": 129.11332231803192,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      "Tue": 147.78926438231792,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      "Wed": 190.90202548253208</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  },</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "week": {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    "ave": 2692.75,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    "std": 261.54588507564023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  }</t>
+  </si>
+  <si>
+    <t>}</t>
+  </si>
+  <si>
+    <t>{"day":{"ave":{"Fri":396.25,"Mon":423.0,"Sat":360.25,"Sun":473.25,"Thu":355.25,"Tue":327.5,"Wed":357.25},"std":{"Fri":88.20572543775148,"Mon":44.7288124888943,"Sat":131.98832801933603,"Sun":120.4778679536896,"Thu":129.11332231803192,"Tue":147.78926438231792,"Wed":190.90202548253208}},"week":{"ave":2692.75,"std":261.54588507564023}}</t>
+  </si>
+  <si>
+    <t>Stats Data</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>400</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (general_error): {"status": "failure", "error": &lt;python error str&gt;, "params": {"start_date": …, "end_date": …}, "response_time_ms": …, "now": …}</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>500</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: { "ok": false, "error": "internal_error", “now”: …, “response_time_ms”: 120}</t>
+    </r>
+  </si>
+  <si>
+    <t>Query params only (both mandatory)</t>
+  </si>
+  <si>
+    <t>{"status": "success", "num_records": 120, "db_connected": true, "params": {"start_date": …, "end_date": …}, "response_time_ms": 120, "now": …, "data": {"day":{"ave":{"Fri":396.25,"Mon":423.0,"Sat":360.25,"Sun":473.25,"Thu":355.25,"Tue":327.5,"Wed":357.25},"std":{"Fri":88.205,"Mon":44.728,"Sat":131.988,"Sun":120.477,"Thu":129.113,"Tue":147.789,"Wed":190.902}},"week":{"ave":2692.75,"std":261.545}}</t>
   </si>
 </sst>
 </file>
@@ -539,7 +673,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -606,6 +740,19 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -660,17 +807,17 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1009,7 +1156,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1055,13 +1202,13 @@
         <v>15</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="F2" s="10" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="87" thickBot="1">
+        <v>27</v>
+      </c>
+      <c r="F2" s="20" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="132.6" thickBot="1">
       <c r="A3" s="6" t="s">
         <v>2</v>
       </c>
@@ -1072,28 +1219,30 @@
         <v>29</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="E3" s="11"/>
-      <c r="F3" s="12" t="s">
-        <v>24</v>
+        <v>60</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="F3" s="19" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="17"/>
-      <c r="B4" s="18"/>
-      <c r="C4" s="19"/>
-      <c r="D4" s="19"/>
-      <c r="E4" s="18"/>
-      <c r="F4" s="20"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="18"/>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="17"/>
-      <c r="B5" s="18"/>
-      <c r="C5" s="19"/>
-      <c r="D5" s="19"/>
-      <c r="E5" s="18"/>
-      <c r="F5" s="20"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="18"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1105,7 +1254,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1220,4 +1369,159 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5746612-BEF7-4CC7-A8C7-B6709CAEDFF6}">
+  <dimension ref="D10:D37"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetData>
+    <row r="10" spans="4:4">
+      <c r="D10" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="11" spans="4:4">
+      <c r="D11" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="12" spans="4:4">
+      <c r="D12" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="4:4">
+      <c r="D13" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="4:4">
+      <c r="D14" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="4:4">
+      <c r="D15" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="16" spans="4:4">
+      <c r="D16" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="17" spans="4:4">
+      <c r="D17" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" spans="4:4">
+      <c r="D18" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="19" spans="4:4">
+      <c r="D19" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="20" spans="4:4">
+      <c r="D20" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="21" spans="4:4">
+      <c r="D21" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="22" spans="4:4">
+      <c r="D22" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="23" spans="4:4">
+      <c r="D23" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="24" spans="4:4">
+      <c r="D24" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="25" spans="4:4">
+      <c r="D25" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="26" spans="4:4">
+      <c r="D26" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="27" spans="4:4">
+      <c r="D27" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="28" spans="4:4">
+      <c r="D28" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="29" spans="4:4">
+      <c r="D29" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="30" spans="4:4">
+      <c r="D30" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="31" spans="4:4">
+      <c r="D31" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="32" spans="4:4">
+      <c r="D32" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="33" spans="4:4">
+      <c r="D33" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="34" spans="4:4">
+      <c r="D34" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="35" spans="4:4">
+      <c r="D35" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="36" spans="4:4">
+      <c r="D36" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="37" spans="4:4">
+      <c r="D37" t="s">
+        <v>55</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
adjusted flask api endpoint schema for /stats
</commit_message>
<xml_diff>
--- a/project_management/flask_apis.xlsx
+++ b/project_management/flask_apis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Grego\Desktop\Coding\Projects\plan_tool\project_management\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F8D781A-CF6D-4D82-81C6-BC75F98BC9B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A21FAC6-88A0-47CA-A6B1-A59F0FC1AD2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{C551EE5F-BC6E-4444-BA40-FE73DEA46AED}"/>
   </bookViews>
@@ -587,6 +587,9 @@
     <t>Stats Data</t>
   </si>
   <si>
+    <t>Query params only (both mandatory)</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <b/>
@@ -606,7 +609,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> (general_error): {"status": "failure", "error": &lt;python error str&gt;, "params": {"start_date": …, "end_date": …}, "response_time_ms": …, "now": …}</t>
+      <t xml:space="preserve"> (general_error): {"ok": True, "error": &lt;python error str&gt;, "response_time_ms": …, "now": …}</t>
     </r>
   </si>
   <si>
@@ -629,14 +632,11 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>: { "ok": false, "error": "internal_error", “now”: …, “response_time_ms”: 120}</t>
-    </r>
-  </si>
-  <si>
-    <t>Query params only (both mandatory)</t>
-  </si>
-  <si>
-    <t>{"status": "success", "num_records": 120, "db_connected": true, "params": {"start_date": …, "end_date": …}, "response_time_ms": 120, "now": …, "data": {"day":{"ave":{"Fri":396.25,"Mon":423.0,"Sat":360.25,"Sun":473.25,"Thu":355.25,"Tue":327.5,"Wed":357.25},"std":{"Fri":88.205,"Mon":44.728,"Sat":131.988,"Sun":120.477,"Thu":129.113,"Tue":147.789,"Wed":190.902}},"week":{"ave":2692.75,"std":261.545}}</t>
+      <t>: { "ok": False, "error": "internal_error", “now”: …, “response_time_ms”: 120}</t>
+    </r>
+  </si>
+  <si>
+    <t>{"ok": True, "num_records": 120, "db_connected": true, "params": {"start_date": …, "end_date": …}, "response_time_ms": 120, "now": …, "data": {"day":{"ave":{"Fri":396.25,"Mon":423.0,"Sat":360.25,"Sun":473.25,"Thu":355.25,"Tue":327.5,"Wed":357.25},"std":{"Fri":88.205,"Mon":44.728,"Sat":131.988,"Sun":120.477,"Thu":129.113,"Tue":147.789,"Wed":190.902}},"week":{"ave":2692.75,"std":261.545}}</t>
   </si>
 </sst>
 </file>
@@ -1156,7 +1156,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1205,7 +1205,7 @@
         <v>27</v>
       </c>
       <c r="F2" s="20" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="132.6" thickBot="1">
@@ -1219,13 +1219,13 @@
         <v>29</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E3" s="11" t="s">
         <v>61</v>
       </c>
       <c r="F3" s="19" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:6">

</xml_diff>

<commit_message>
added /api/db/health + /api/notion/health schemas to documentation
</commit_message>
<xml_diff>
--- a/project_management/flask_apis.xlsx
+++ b/project_management/flask_apis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Grego\Desktop\Coding\Projects\plan_tool\project_management\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A21FAC6-88A0-47CA-A6B1-A59F0FC1AD2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E6B63DB-75F6-4622-A7FA-96384249C2B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{C551EE5F-BC6E-4444-BA40-FE73DEA46AED}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="67">
   <si>
     <t>Method</t>
   </si>
@@ -590,6 +590,27 @@
     <t>Query params only (both mandatory)</t>
   </si>
   <si>
+    <t>503: { "ok": False, "error": "internal_error", “now”: …, “response_time_ms”: 120}</t>
+  </si>
+  <si>
+    <t>200: { "ok": true, "service": "flask", "version": "x.y.z", "now": "2025-08-23T17:02:00Z" }</t>
+  </si>
+  <si>
+    <t>200: {"ok": True, "num_records": 120, "db_connected": true, "params": {"start_date": …, "end_date": …}, "response_time_ms": 120, "now": …, "data": {"day":{"ave":{"Fri":396.25,"Mon":423.0,"Sat":360.25,"Sun":473.25,"Thu":355.25,"Tue":327.5,"Wed":357.25},"std":{"Fri":88.205,"Mon":44.728,"Sat":131.988,"Sun":120.477,"Thu":129.113,"Tue":147.789,"Wed":190.902}},"week":{"ave":2692.75,"std":261.545}}</t>
+  </si>
+  <si>
+    <t>Test to see if notion is working</t>
+  </si>
+  <si>
+    <t>Test to see if database (supabase) is working</t>
+  </si>
+  <si>
+    <t>200: {"ok": True, "user": "…", "now": "…", "response_time_ms": 102, "service": "notion", "version": "…"}</t>
+  </si>
+  <si>
+    <t>200: {"ok": True, "now": "…", "response_time_ms": 102, "service": "supabase", "version": "…"}</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <b/>
@@ -599,44 +620,18 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>400</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> (general_error): {"ok": True, "error": &lt;python error str&gt;, "response_time_ms": …, "now": …}</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>500</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>: { "ok": False, "error": "internal_error", “now”: …, “response_time_ms”: 120}</t>
-    </r>
-  </si>
-  <si>
-    <t>{"ok": True, "num_records": 120, "db_connected": true, "params": {"start_date": …, "end_date": …}, "response_time_ms": 120, "now": …, "data": {"day":{"ave":{"Fri":396.25,"Mon":423.0,"Sat":360.25,"Sun":473.25,"Thu":355.25,"Tue":327.5,"Wed":357.25},"std":{"Fri":88.205,"Mon":44.728,"Sat":131.988,"Sun":120.477,"Thu":129.113,"Tue":147.789,"Wed":190.902}},"week":{"ave":2692.75,"std":261.545}}</t>
+      <t>503</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (general_error): {"ok": False, "error": &lt;python error str&gt;, "response_time_ms": …, "now": …}</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1153,10 +1148,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D880C055-EB2C-4AF6-84A3-82DF6903CA3E}">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1189,60 +1184,102 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="29.4" thickBot="1">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>27</v>
+      <c r="E2" s="11" t="s">
+        <v>60</v>
       </c>
       <c r="F2" s="20" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="132.6" thickBot="1">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="40.200000000000003" thickBot="1">
       <c r="A3" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="9" t="str">
+        <f>"/api/notion/health"</f>
+        <v>/api/notion/health</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="F3" s="20" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="40.200000000000003" thickBot="1">
+      <c r="A4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="5" t="str">
+        <f>"/api/db/health"</f>
+        <v>/api/db/health</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="F4" s="20" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="132.6" thickBot="1">
+      <c r="A5" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C5" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D5" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="E3" s="11" t="s">
+      <c r="E5" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="F3" s="19" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" s="17"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="18"/>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" s="17"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="18"/>
+      <c r="F5" s="19" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="17"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="18"/>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="17"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="18"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added 7th standup log for sprint 8 + updated flask_api.xlsx documentation file
</commit_message>
<xml_diff>
--- a/project_management/flask_apis.xlsx
+++ b/project_management/flask_apis.xlsx
@@ -5,17 +5,16 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Grego\Desktop\Coding\Projects\plan_tool\project_management\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Grego\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E6B63DB-75F6-4622-A7FA-96384249C2B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE8BEF37-E430-4A05-AF75-B1F2A8DC73EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{C551EE5F-BC6E-4444-BA40-FE73DEA46AED}"/>
   </bookViews>
   <sheets>
     <sheet name="api_doc" sheetId="4" r:id="rId1"/>
     <sheet name="design_1" sheetId="5" r:id="rId2"/>
-    <sheet name="stats_data_example" sheetId="7" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="40">
   <si>
     <t>Method</t>
   </si>
@@ -503,114 +502,12 @@
     <t>Request statistical metric calculations that will filter work records based on the start and end date values passed (inclusive)</t>
   </si>
   <si>
-    <t>{</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  "day": {</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    "ave": {</t>
-  </si>
-  <si>
-    <t xml:space="preserve">      "Fri": 396.25,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">      "Mon": 423.0,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">      "Sat": 360.25,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">      "Sun": 473.25,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">      "Thu": 355.25,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">      "Tue": 327.5,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">      "Wed": 357.25</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    },</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    "std": {</t>
-  </si>
-  <si>
-    <t xml:space="preserve">      "Fri": 88.20572543775148,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">      "Mon": 44.7288124888943,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">      "Sat": 131.98832801933603,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">      "Sun": 120.4778679536896,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">      "Thu": 129.11332231803192,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">      "Tue": 147.78926438231792,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">      "Wed": 190.90202548253208</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    }</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  },</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  "week": {</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    "ave": 2692.75,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    "std": 261.54588507564023</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  }</t>
-  </si>
-  <si>
-    <t>}</t>
-  </si>
-  <si>
-    <t>{"day":{"ave":{"Fri":396.25,"Mon":423.0,"Sat":360.25,"Sun":473.25,"Thu":355.25,"Tue":327.5,"Wed":357.25},"std":{"Fri":88.20572543775148,"Mon":44.7288124888943,"Sat":131.98832801933603,"Sun":120.4778679536896,"Thu":129.11332231803192,"Tue":147.78926438231792,"Wed":190.90202548253208}},"week":{"ave":2692.75,"std":261.54588507564023}}</t>
-  </si>
-  <si>
-    <t>Stats Data</t>
-  </si>
-  <si>
     <t>Query params only (both mandatory)</t>
   </si>
   <si>
-    <t>503: { "ok": False, "error": "internal_error", “now”: …, “response_time_ms”: 120}</t>
-  </si>
-  <si>
-    <t>200: { "ok": true, "service": "flask", "version": "x.y.z", "now": "2025-08-23T17:02:00Z" }</t>
-  </si>
-  <si>
-    <t>200: {"ok": True, "num_records": 120, "db_connected": true, "params": {"start_date": …, "end_date": …}, "response_time_ms": 120, "now": …, "data": {"day":{"ave":{"Fri":396.25,"Mon":423.0,"Sat":360.25,"Sun":473.25,"Thu":355.25,"Tue":327.5,"Wed":357.25},"std":{"Fri":88.205,"Mon":44.728,"Sat":131.988,"Sun":120.477,"Thu":129.113,"Tue":147.789,"Wed":190.902}},"week":{"ave":2692.75,"std":261.545}}</t>
-  </si>
-  <si>
     <t>Test to see if notion is working</t>
   </si>
   <si>
-    <t>Test to see if database (supabase) is working</t>
-  </si>
-  <si>
-    <t>200: {"ok": True, "user": "…", "now": "…", "response_time_ms": 102, "service": "notion", "version": "…"}</t>
-  </si>
-  <si>
-    <t>200: {"ok": True, "now": "…", "response_time_ms": 102, "service": "supabase", "version": "…"}</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <b/>
@@ -630,15 +527,224 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> (general_error): {"ok": False, "error": &lt;python error str&gt;, "response_time_ms": …, "now": …}</t>
-    </r>
+      <t xml:space="preserve">: { "ok": false, "service": "notion", "version": "2022-06-28", "now": "…Z", "response_time_ms": 312.9, "checks": { "user": { "ok": false, "status_code": 401 }, "database": { "ok": true, "status_code": 200 } }, "error": "Network Error: Notion user inaccessible" }, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>503</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: { "ok": false, "service": "notion", "version": "2022-06-28", "now": "…Z", "response_time_ms": 300, "checks": { "user": { "ok": true, "status_code": 200 }, "database": { "ok": false, "status_code": 404 } }, "error": "Network Error: Notion database inaccessible" }, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>503</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: { "ok": false, "service": "notion", "version": "2022-06-28", "now": "…Z", "response_time_ms": 290, "checks": { "user": { "ok": false, "status_code": 401 }, "database": { "ok": false, "status_code": 404 } }, "error": "Network Error: Notion user AND database inaccessible" }, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>503</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: { "ok": false, "service": "notion", "version": "2022-06-28", "now": "…Z", "response_time_ms": 200, "error": "network_error" }, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>500</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: { "ok": false, "service": "notion", "version": "2022-06-28", "now": "…Z", "response_time_ms": 500, "error": "internal_error" }</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>503</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: { "ok": False, "error": "internal_error", “now”: …, “response_time_ms”: 120}</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>503:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> { "ok": false, "error": "internal_error", "response_time_ms": 150, "now": "…Z" }</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>200</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t xml:space="preserve">: { "ok": true, "service": "notion", "version": "2022-06-28", "now": "…Z", "response_time_ms": 143.2, "checks": { "user": { "ok": true, "status_code": 200 }, "database": { "ok": true, "status_code": 200 } } } </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>200</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>: { "ok": true, "num_records": 42, "db_connected": true, "params": { "start_date": "YYYY-MM-DD", "end_date": "YYYY-MM-DD" }, "response_time_ms": 220, "now": "…Z", "data": { "week": { … }, "day": { … } } }</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>200</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>: {"ok": True, "user": "…", "now": "…", "response_time_ms": 102, "service": "notion", "version": "…"}</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>200</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>: { "ok": true, "service": "flask", "version": "x.y.z", "now": "2025-08-23T17:02:00Z" }</t>
+    </r>
+  </si>
+  <si>
+    <t>Test to see if database (supabase) is working. Queries both my user account and the target database</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -655,6 +761,12 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
+    </font>
+    <font>
+      <b/>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial Unicode MS"/>
@@ -752,7 +864,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -813,6 +925,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1151,7 +1266,7 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1160,7 +1275,7 @@
     <col min="3" max="3" width="20.44140625" customWidth="1"/>
     <col min="4" max="4" width="28" customWidth="1"/>
     <col min="5" max="5" width="38.21875" customWidth="1"/>
-    <col min="6" max="6" width="51" customWidth="1"/>
+    <col min="6" max="6" width="67" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15" thickBot="1">
@@ -1197,10 +1312,10 @@
         <v>15</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>60</v>
+        <v>38</v>
       </c>
       <c r="F2" s="20" t="s">
-        <v>59</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="40.200000000000003" thickBot="1">
@@ -1212,19 +1327,19 @@
         <v>/api/notion/health</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>62</v>
+        <v>31</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>15</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>64</v>
+        <v>37</v>
       </c>
       <c r="F3" s="20" t="s">
-        <v>59</v>
+        <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="40.200000000000003" thickBot="1">
+    <row r="4" spans="1:6" ht="202.2" thickBot="1">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -1233,19 +1348,19 @@
         <v>/api/db/health</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>63</v>
+        <v>39</v>
       </c>
       <c r="D4" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="11" t="s">
-        <v>65</v>
+      <c r="E4" s="21" t="s">
+        <v>35</v>
       </c>
       <c r="F4" s="20" t="s">
-        <v>59</v>
+        <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="132.6" thickBot="1">
+    <row r="5" spans="1:6" ht="87" thickBot="1">
       <c r="A5" s="6" t="s">
         <v>2</v>
       </c>
@@ -1256,13 +1371,13 @@
         <v>29</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>58</v>
+        <v>30</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>61</v>
+        <v>36</v>
       </c>
       <c r="F5" s="19" t="s">
-        <v>66</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -1406,159 +1521,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5746612-BEF7-4CC7-A8C7-B6709CAEDFF6}">
-  <dimension ref="D10:D37"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
-  <sheetData>
-    <row r="10" spans="4:4">
-      <c r="D10" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="11" spans="4:4">
-      <c r="D11" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="12" spans="4:4">
-      <c r="D12" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="13" spans="4:4">
-      <c r="D13" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="14" spans="4:4">
-      <c r="D14" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="15" spans="4:4">
-      <c r="D15" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="16" spans="4:4">
-      <c r="D16" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="17" spans="4:4">
-      <c r="D17" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="18" spans="4:4">
-      <c r="D18" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="19" spans="4:4">
-      <c r="D19" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="20" spans="4:4">
-      <c r="D20" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="21" spans="4:4">
-      <c r="D21" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="22" spans="4:4">
-      <c r="D22" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="23" spans="4:4">
-      <c r="D23" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="24" spans="4:4">
-      <c r="D24" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="25" spans="4:4">
-      <c r="D25" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="26" spans="4:4">
-      <c r="D26" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="27" spans="4:4">
-      <c r="D27" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="28" spans="4:4">
-      <c r="D28" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="29" spans="4:4">
-      <c r="D29" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="30" spans="4:4">
-      <c r="D30" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="31" spans="4:4">
-      <c r="D31" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="32" spans="4:4">
-      <c r="D32" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="33" spans="4:4">
-      <c r="D33" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="34" spans="4:4">
-      <c r="D34" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="35" spans="4:4">
-      <c r="D35" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="36" spans="4:4">
-      <c r="D36" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="37" spans="4:4">
-      <c r="D37" t="s">
-        <v>55</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>